<commit_message>
update column names in rodent_test_data
</commit_message>
<xml_diff>
--- a/DataCleaningScripts/rodent_test_data.xlsx
+++ b/DataCleaningScripts/rodent_test_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EC\Desktop\git\PortalData\DataCleaningScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11985" windowHeight="15375" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11988" windowHeight="15372" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EKB" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="386">
   <si>
     <t>mo</t>
   </si>
@@ -1175,6 +1175,15 @@
   </si>
   <si>
     <t>B267EB</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -1610,30 +1619,30 @@
       <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.9" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.109375" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.42578125" customWidth="1"/>
+    <col min="6" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.44140625" customWidth="1"/>
     <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1719,7 +1728,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>7</v>
       </c>
@@ -1758,7 +1767,7 @@
       </c>
       <c r="U2"/>
     </row>
-    <row r="3" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7</v>
       </c>
@@ -1794,7 +1803,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7</v>
       </c>
@@ -1833,7 +1842,7 @@
       </c>
       <c r="U4"/>
     </row>
-    <row r="5" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -1869,7 +1878,7 @@
       </c>
       <c r="U5"/>
     </row>
-    <row r="6" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
@@ -1908,7 +1917,7 @@
       </c>
       <c r="U6"/>
     </row>
-    <row r="7" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1947,7 +1956,7 @@
       </c>
       <c r="U7"/>
     </row>
-    <row r="8" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1986,7 +1995,7 @@
       </c>
       <c r="U8"/>
     </row>
-    <row r="9" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2025,7 +2034,7 @@
       </c>
       <c r="U9"/>
     </row>
-    <row r="10" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2064,7 +2073,7 @@
       </c>
       <c r="U10"/>
     </row>
-    <row r="11" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2100,7 +2109,7 @@
       </c>
       <c r="U11"/>
     </row>
-    <row r="12" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
@@ -2139,7 +2148,7 @@
       </c>
       <c r="U12"/>
     </row>
-    <row r="13" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -2181,7 +2190,7 @@
       </c>
       <c r="U13"/>
     </row>
-    <row r="14" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -2220,7 +2229,7 @@
       </c>
       <c r="U14"/>
     </row>
-    <row r="15" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -2256,7 +2265,7 @@
       </c>
       <c r="U15"/>
     </row>
-    <row r="16" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
@@ -2295,7 +2304,7 @@
       </c>
       <c r="U16"/>
     </row>
-    <row r="17" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7</v>
       </c>
@@ -2334,7 +2343,7 @@
       </c>
       <c r="U17"/>
     </row>
-    <row r="18" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7</v>
       </c>
@@ -2373,7 +2382,7 @@
       </c>
       <c r="U18"/>
     </row>
-    <row r="19" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
@@ -2412,7 +2421,7 @@
       </c>
       <c r="U19"/>
     </row>
-    <row r="20" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -2451,7 +2460,7 @@
       </c>
       <c r="U20"/>
     </row>
-    <row r="21" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
@@ -2490,7 +2499,7 @@
       </c>
       <c r="U21"/>
     </row>
-    <row r="22" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
@@ -2529,7 +2538,7 @@
       </c>
       <c r="U22"/>
     </row>
-    <row r="23" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7</v>
       </c>
@@ -2568,7 +2577,7 @@
       </c>
       <c r="U23"/>
     </row>
-    <row r="24" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>7</v>
       </c>
@@ -2607,7 +2616,7 @@
       </c>
       <c r="U24"/>
     </row>
-    <row r="25" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7</v>
       </c>
@@ -2646,7 +2655,7 @@
       </c>
       <c r="U25"/>
     </row>
-    <row r="26" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>7</v>
       </c>
@@ -2685,7 +2694,7 @@
       </c>
       <c r="U26"/>
     </row>
-    <row r="27" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7</v>
       </c>
@@ -2724,7 +2733,7 @@
       </c>
       <c r="U27"/>
     </row>
-    <row r="28" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7</v>
       </c>
@@ -2763,7 +2772,7 @@
       </c>
       <c r="U28"/>
     </row>
-    <row r="29" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7</v>
       </c>
@@ -2802,7 +2811,7 @@
       </c>
       <c r="U29"/>
     </row>
-    <row r="30" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>7</v>
       </c>
@@ -2841,7 +2850,7 @@
       </c>
       <c r="U30"/>
     </row>
-    <row r="31" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7</v>
       </c>
@@ -2880,7 +2889,7 @@
       </c>
       <c r="U31"/>
     </row>
-    <row r="32" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7</v>
       </c>
@@ -2919,7 +2928,7 @@
       </c>
       <c r="U32"/>
     </row>
-    <row r="33" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7</v>
       </c>
@@ -2958,7 +2967,7 @@
       </c>
       <c r="U33"/>
     </row>
-    <row r="34" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7</v>
       </c>
@@ -3000,7 +3009,7 @@
       </c>
       <c r="U34"/>
     </row>
-    <row r="35" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7</v>
       </c>
@@ -3039,7 +3048,7 @@
       </c>
       <c r="U35"/>
     </row>
-    <row r="36" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7</v>
       </c>
@@ -3078,7 +3087,7 @@
       </c>
       <c r="U36"/>
     </row>
-    <row r="37" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>7</v>
       </c>
@@ -3117,7 +3126,7 @@
       </c>
       <c r="U37"/>
     </row>
-    <row r="38" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7</v>
       </c>
@@ -3159,7 +3168,7 @@
       </c>
       <c r="U38"/>
     </row>
-    <row r="39" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>7</v>
       </c>
@@ -3198,7 +3207,7 @@
       </c>
       <c r="U39"/>
     </row>
-    <row r="40" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7</v>
       </c>
@@ -3237,7 +3246,7 @@
       </c>
       <c r="U40"/>
     </row>
-    <row r="41" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>7</v>
       </c>
@@ -3276,7 +3285,7 @@
       </c>
       <c r="U41"/>
     </row>
-    <row r="42" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7</v>
       </c>
@@ -3318,7 +3327,7 @@
       </c>
       <c r="U42"/>
     </row>
-    <row r="43" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7</v>
       </c>
@@ -3360,7 +3369,7 @@
       </c>
       <c r="U43"/>
     </row>
-    <row r="44" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>7</v>
       </c>
@@ -3405,7 +3414,7 @@
       </c>
       <c r="U44"/>
     </row>
-    <row r="45" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>7</v>
       </c>
@@ -3444,7 +3453,7 @@
       </c>
       <c r="U45"/>
     </row>
-    <row r="46" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>7</v>
       </c>
@@ -3483,7 +3492,7 @@
       </c>
       <c r="U46"/>
     </row>
-    <row r="47" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>7</v>
       </c>
@@ -3525,7 +3534,7 @@
       </c>
       <c r="U47"/>
     </row>
-    <row r="48" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>7</v>
       </c>
@@ -3564,7 +3573,7 @@
       </c>
       <c r="U48"/>
     </row>
-    <row r="49" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7</v>
       </c>
@@ -3603,7 +3612,7 @@
       </c>
       <c r="U49"/>
     </row>
-    <row r="50" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>7</v>
       </c>
@@ -3645,7 +3654,7 @@
       </c>
       <c r="U50"/>
     </row>
-    <row r="51" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>7</v>
       </c>
@@ -3684,7 +3693,7 @@
       </c>
       <c r="U51"/>
     </row>
-    <row r="52" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>7</v>
       </c>
@@ -3723,7 +3732,7 @@
       </c>
       <c r="U52"/>
     </row>
-    <row r="53" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>7</v>
       </c>
@@ -3765,7 +3774,7 @@
       </c>
       <c r="U53"/>
     </row>
-    <row r="54" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>7</v>
       </c>
@@ -3807,7 +3816,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>7</v>
       </c>
@@ -3846,7 +3855,7 @@
       </c>
       <c r="U55"/>
     </row>
-    <row r="56" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>7</v>
       </c>
@@ -3885,7 +3894,7 @@
       </c>
       <c r="U56"/>
     </row>
-    <row r="57" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>7</v>
       </c>
@@ -3924,7 +3933,7 @@
       </c>
       <c r="U57"/>
     </row>
-    <row r="58" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>7</v>
       </c>
@@ -3966,7 +3975,7 @@
       </c>
       <c r="U58"/>
     </row>
-    <row r="59" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>7</v>
       </c>
@@ -4005,7 +4014,7 @@
       </c>
       <c r="U59"/>
     </row>
-    <row r="60" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>7</v>
       </c>
@@ -4044,7 +4053,7 @@
       </c>
       <c r="U60"/>
     </row>
-    <row r="61" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>7</v>
       </c>
@@ -4083,7 +4092,7 @@
       </c>
       <c r="U61"/>
     </row>
-    <row r="62" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>7</v>
       </c>
@@ -4122,7 +4131,7 @@
       </c>
       <c r="U62"/>
     </row>
-    <row r="63" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>7</v>
       </c>
@@ -4161,7 +4170,7 @@
       </c>
       <c r="U63"/>
     </row>
-    <row r="64" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>7</v>
       </c>
@@ -4200,7 +4209,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>7</v>
       </c>
@@ -4242,7 +4251,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>7</v>
       </c>
@@ -4281,7 +4290,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>7</v>
       </c>
@@ -4320,7 +4329,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>7</v>
       </c>
@@ -4359,7 +4368,7 @@
       </c>
       <c r="U68"/>
     </row>
-    <row r="69" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>7</v>
       </c>
@@ -4398,7 +4407,7 @@
       </c>
       <c r="U69"/>
     </row>
-    <row r="70" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>7</v>
       </c>
@@ -4437,7 +4446,7 @@
       </c>
       <c r="U70"/>
     </row>
-    <row r="71" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>7</v>
       </c>
@@ -4476,7 +4485,7 @@
       </c>
       <c r="U71"/>
     </row>
-    <row r="72" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>7</v>
       </c>
@@ -4515,7 +4524,7 @@
       </c>
       <c r="U72"/>
     </row>
-    <row r="73" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>7</v>
       </c>
@@ -4554,7 +4563,7 @@
       </c>
       <c r="U73"/>
     </row>
-    <row r="74" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>7</v>
       </c>
@@ -4596,7 +4605,7 @@
       </c>
       <c r="U74"/>
     </row>
-    <row r="75" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>7</v>
       </c>
@@ -4638,7 +4647,7 @@
       </c>
       <c r="U75"/>
     </row>
-    <row r="76" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>7</v>
       </c>
@@ -4677,7 +4686,7 @@
       </c>
       <c r="U76"/>
     </row>
-    <row r="77" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>7</v>
       </c>
@@ -4716,7 +4725,7 @@
       </c>
       <c r="U77"/>
     </row>
-    <row r="78" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>7</v>
       </c>
@@ -4755,7 +4764,7 @@
       </c>
       <c r="U78"/>
     </row>
-    <row r="79" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>7</v>
       </c>
@@ -4794,7 +4803,7 @@
       </c>
       <c r="U79"/>
     </row>
-    <row r="80" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>7</v>
       </c>
@@ -4836,7 +4845,7 @@
       </c>
       <c r="U80"/>
     </row>
-    <row r="81" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>7</v>
       </c>
@@ -4875,7 +4884,7 @@
       </c>
       <c r="U81"/>
     </row>
-    <row r="82" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>7</v>
       </c>
@@ -4914,7 +4923,7 @@
       </c>
       <c r="U82"/>
     </row>
-    <row r="83" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>7</v>
       </c>
@@ -4956,7 +4965,7 @@
       </c>
       <c r="U83"/>
     </row>
-    <row r="84" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>7</v>
       </c>
@@ -4995,7 +5004,7 @@
       </c>
       <c r="U84"/>
     </row>
-    <row r="85" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>7</v>
       </c>
@@ -5034,7 +5043,7 @@
       </c>
       <c r="U85"/>
     </row>
-    <row r="86" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>7</v>
       </c>
@@ -5073,7 +5082,7 @@
       </c>
       <c r="U86"/>
     </row>
-    <row r="87" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>7</v>
       </c>
@@ -5112,7 +5121,7 @@
       </c>
       <c r="U87"/>
     </row>
-    <row r="88" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>7</v>
       </c>
@@ -5151,7 +5160,7 @@
       </c>
       <c r="U88"/>
     </row>
-    <row r="89" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>7</v>
       </c>
@@ -5190,7 +5199,7 @@
       </c>
       <c r="U89"/>
     </row>
-    <row r="90" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>7</v>
       </c>
@@ -5229,7 +5238,7 @@
       </c>
       <c r="U90"/>
     </row>
-    <row r="91" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>7</v>
       </c>
@@ -5268,7 +5277,7 @@
       </c>
       <c r="U91"/>
     </row>
-    <row r="92" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>7</v>
       </c>
@@ -5307,7 +5316,7 @@
       </c>
       <c r="U92"/>
     </row>
-    <row r="93" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>7</v>
       </c>
@@ -5346,7 +5355,7 @@
       </c>
       <c r="U93"/>
     </row>
-    <row r="94" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>7</v>
       </c>
@@ -5385,7 +5394,7 @@
       </c>
       <c r="U94"/>
     </row>
-    <row r="95" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>7</v>
       </c>
@@ -5427,7 +5436,7 @@
       </c>
       <c r="U95"/>
     </row>
-    <row r="96" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>7</v>
       </c>
@@ -5469,7 +5478,7 @@
       </c>
       <c r="U96"/>
     </row>
-    <row r="97" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>7</v>
       </c>
@@ -5508,7 +5517,7 @@
       </c>
       <c r="U97"/>
     </row>
-    <row r="98" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>7</v>
       </c>
@@ -5547,7 +5556,7 @@
       </c>
       <c r="U98"/>
     </row>
-    <row r="99" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>7</v>
       </c>
@@ -5589,7 +5598,7 @@
       </c>
       <c r="U99"/>
     </row>
-    <row r="100" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>7</v>
       </c>
@@ -5631,7 +5640,7 @@
       </c>
       <c r="U100"/>
     </row>
-    <row r="101" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>7</v>
       </c>
@@ -5670,7 +5679,7 @@
       </c>
       <c r="U101"/>
     </row>
-    <row r="102" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>7</v>
       </c>
@@ -5709,7 +5718,7 @@
       </c>
       <c r="U102"/>
     </row>
-    <row r="103" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>7</v>
       </c>
@@ -5751,7 +5760,7 @@
       </c>
       <c r="U103"/>
     </row>
-    <row r="104" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>7</v>
       </c>
@@ -5790,7 +5799,7 @@
       </c>
       <c r="U104"/>
     </row>
-    <row r="105" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>7</v>
       </c>
@@ -5829,7 +5838,7 @@
       </c>
       <c r="U105"/>
     </row>
-    <row r="106" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>7</v>
       </c>
@@ -5868,7 +5877,7 @@
       </c>
       <c r="U106"/>
     </row>
-    <row r="107" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>7</v>
       </c>
@@ -5907,7 +5916,7 @@
       </c>
       <c r="U107"/>
     </row>
-    <row r="108" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>7</v>
       </c>
@@ -5949,7 +5958,7 @@
       </c>
       <c r="U108"/>
     </row>
-    <row r="109" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>7</v>
       </c>
@@ -5988,7 +5997,7 @@
       </c>
       <c r="U109"/>
     </row>
-    <row r="110" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>7</v>
       </c>
@@ -6027,7 +6036,7 @@
       </c>
       <c r="U110"/>
     </row>
-    <row r="111" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>7</v>
       </c>
@@ -6066,7 +6075,7 @@
       </c>
       <c r="U111"/>
     </row>
-    <row r="112" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>7</v>
       </c>
@@ -6105,7 +6114,7 @@
       </c>
       <c r="U112"/>
     </row>
-    <row r="113" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>7</v>
       </c>
@@ -6144,7 +6153,7 @@
       </c>
       <c r="U113"/>
     </row>
-    <row r="114" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>7</v>
       </c>
@@ -6186,7 +6195,7 @@
       </c>
       <c r="U114"/>
     </row>
-    <row r="115" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>7</v>
       </c>
@@ -6228,7 +6237,7 @@
       </c>
       <c r="U115"/>
     </row>
-    <row r="116" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>7</v>
       </c>
@@ -6270,7 +6279,7 @@
       </c>
       <c r="U116"/>
     </row>
-    <row r="117" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>7</v>
       </c>
@@ -6309,7 +6318,7 @@
       </c>
       <c r="U117"/>
     </row>
-    <row r="118" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>7</v>
       </c>
@@ -6348,7 +6357,7 @@
       </c>
       <c r="U118"/>
     </row>
-    <row r="119" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>7</v>
       </c>
@@ -6387,7 +6396,7 @@
       </c>
       <c r="U119"/>
     </row>
-    <row r="120" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>7</v>
       </c>
@@ -6426,7 +6435,7 @@
       </c>
       <c r="U120"/>
     </row>
-    <row r="121" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>7</v>
       </c>
@@ -6465,7 +6474,7 @@
       </c>
       <c r="U121"/>
     </row>
-    <row r="122" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>7</v>
       </c>
@@ -6504,7 +6513,7 @@
       </c>
       <c r="U122"/>
     </row>
-    <row r="123" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>7</v>
       </c>
@@ -6543,7 +6552,7 @@
       </c>
       <c r="U123"/>
     </row>
-    <row r="124" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>7</v>
       </c>
@@ -6585,7 +6594,7 @@
       </c>
       <c r="U124"/>
     </row>
-    <row r="125" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>7</v>
       </c>
@@ -6627,7 +6636,7 @@
       </c>
       <c r="U125"/>
     </row>
-    <row r="126" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>7</v>
       </c>
@@ -6666,7 +6675,7 @@
       </c>
       <c r="U126"/>
     </row>
-    <row r="127" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>7</v>
       </c>
@@ -6705,7 +6714,7 @@
       </c>
       <c r="U127"/>
     </row>
-    <row r="128" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>7</v>
       </c>
@@ -6744,7 +6753,7 @@
       </c>
       <c r="U128"/>
     </row>
-    <row r="129" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>7</v>
       </c>
@@ -6786,7 +6795,7 @@
       </c>
       <c r="U129"/>
     </row>
-    <row r="130" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>7</v>
       </c>
@@ -6828,7 +6837,7 @@
       </c>
       <c r="U130"/>
     </row>
-    <row r="131" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>7</v>
       </c>
@@ -6867,7 +6876,7 @@
       </c>
       <c r="U131"/>
     </row>
-    <row r="132" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>7</v>
       </c>
@@ -6909,7 +6918,7 @@
       </c>
       <c r="U132"/>
     </row>
-    <row r="133" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>7</v>
       </c>
@@ -6936,7 +6945,7 @@
       </c>
       <c r="U133"/>
     </row>
-    <row r="134" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>7</v>
       </c>
@@ -6978,7 +6987,7 @@
       </c>
       <c r="U134"/>
     </row>
-    <row r="135" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>7</v>
       </c>
@@ -7017,7 +7026,7 @@
       </c>
       <c r="U135"/>
     </row>
-    <row r="136" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>7</v>
       </c>
@@ -7056,7 +7065,7 @@
       </c>
       <c r="U136"/>
     </row>
-    <row r="137" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>7</v>
       </c>
@@ -7095,7 +7104,7 @@
       </c>
       <c r="U137"/>
     </row>
-    <row r="138" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>7</v>
       </c>
@@ -7134,7 +7143,7 @@
       </c>
       <c r="U138"/>
     </row>
-    <row r="139" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>7</v>
       </c>
@@ -7176,7 +7185,7 @@
       </c>
       <c r="U139"/>
     </row>
-    <row r="140" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>7</v>
       </c>
@@ -7215,7 +7224,7 @@
       </c>
       <c r="U140"/>
     </row>
-    <row r="141" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>7</v>
       </c>
@@ -7260,7 +7269,7 @@
       </c>
       <c r="U141"/>
     </row>
-    <row r="142" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>7</v>
       </c>
@@ -7302,7 +7311,7 @@
       </c>
       <c r="U142"/>
     </row>
-    <row r="143" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>7</v>
       </c>
@@ -7341,7 +7350,7 @@
       </c>
       <c r="U143"/>
     </row>
-    <row r="144" spans="1:21" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:21" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>7</v>
       </c>
@@ -7380,7 +7389,7 @@
       </c>
       <c r="U144"/>
     </row>
-    <row r="145" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>7</v>
       </c>
@@ -7422,7 +7431,7 @@
       </c>
       <c r="U145"/>
     </row>
-    <row r="146" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>7</v>
       </c>
@@ -7464,7 +7473,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="147" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>7</v>
       </c>
@@ -7506,7 +7515,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="148" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>7</v>
       </c>
@@ -7545,7 +7554,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="149" spans="1:28" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:28" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>7</v>
       </c>
@@ -7670,41 +7679,41 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q41" sqref="Q41"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.109375" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.42578125" customWidth="1"/>
+    <col min="6" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.44140625" customWidth="1"/>
     <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>383</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>384</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>385</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -7782,7 +7791,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>7</v>
       </c>
@@ -7821,7 +7830,7 @@
       </c>
       <c r="U2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7</v>
       </c>
@@ -7857,7 +7866,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7</v>
       </c>
@@ -7896,7 +7905,7 @@
       </c>
       <c r="U4"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -7932,7 +7941,7 @@
       </c>
       <c r="U5"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
@@ -7971,7 +7980,7 @@
       </c>
       <c r="U6"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -8010,7 +8019,7 @@
       </c>
       <c r="U7"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -8049,7 +8058,7 @@
       </c>
       <c r="U8"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -8088,7 +8097,7 @@
       </c>
       <c r="U9"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -8127,7 +8136,7 @@
       </c>
       <c r="U10"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -8163,7 +8172,7 @@
       </c>
       <c r="U11"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
@@ -8202,7 +8211,7 @@
       </c>
       <c r="U12"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -8244,7 +8253,7 @@
       </c>
       <c r="U13"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -8283,7 +8292,7 @@
       </c>
       <c r="U14"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -8319,7 +8328,7 @@
       </c>
       <c r="U15"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
@@ -8358,7 +8367,7 @@
       </c>
       <c r="U16"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7</v>
       </c>
@@ -8397,7 +8406,7 @@
       </c>
       <c r="U17"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7</v>
       </c>
@@ -8436,7 +8445,7 @@
       </c>
       <c r="U18"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
@@ -8475,7 +8484,7 @@
       </c>
       <c r="U19"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -8514,7 +8523,7 @@
       </c>
       <c r="U20"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
@@ -8553,7 +8562,7 @@
       </c>
       <c r="U21"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
@@ -8592,7 +8601,7 @@
       </c>
       <c r="U22"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7</v>
       </c>
@@ -8631,7 +8640,7 @@
       </c>
       <c r="U23"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>7</v>
       </c>
@@ -8670,7 +8679,7 @@
       </c>
       <c r="U24"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7</v>
       </c>
@@ -8709,7 +8718,7 @@
       </c>
       <c r="U25"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>7</v>
       </c>
@@ -8748,7 +8757,7 @@
       </c>
       <c r="U26"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7</v>
       </c>
@@ -8787,7 +8796,7 @@
       </c>
       <c r="U27"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7</v>
       </c>
@@ -8826,7 +8835,7 @@
       </c>
       <c r="U28"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7</v>
       </c>
@@ -8865,7 +8874,7 @@
       </c>
       <c r="U29"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>7</v>
       </c>
@@ -8904,7 +8913,7 @@
       </c>
       <c r="U30"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7</v>
       </c>
@@ -8943,7 +8952,7 @@
       </c>
       <c r="U31"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7</v>
       </c>
@@ -8982,7 +8991,7 @@
       </c>
       <c r="U32"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7</v>
       </c>
@@ -9021,7 +9030,7 @@
       </c>
       <c r="U33"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7</v>
       </c>
@@ -9063,7 +9072,7 @@
       </c>
       <c r="U34"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7</v>
       </c>
@@ -9102,7 +9111,7 @@
       </c>
       <c r="U35"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7</v>
       </c>
@@ -9141,7 +9150,7 @@
       </c>
       <c r="U36"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>7</v>
       </c>
@@ -9180,7 +9189,7 @@
       </c>
       <c r="U37"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7</v>
       </c>
@@ -9222,7 +9231,7 @@
       </c>
       <c r="U38"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>7</v>
       </c>
@@ -9261,7 +9270,7 @@
       </c>
       <c r="U39"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7</v>
       </c>
@@ -9300,7 +9309,7 @@
       </c>
       <c r="U40"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>7</v>
       </c>
@@ -9339,7 +9348,7 @@
       </c>
       <c r="U41"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7</v>
       </c>
@@ -9381,7 +9390,7 @@
       </c>
       <c r="U42"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7</v>
       </c>
@@ -9423,7 +9432,7 @@
       </c>
       <c r="U43"/>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>7</v>
       </c>
@@ -9468,7 +9477,7 @@
       </c>
       <c r="U44"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>7</v>
       </c>
@@ -9507,7 +9516,7 @@
       </c>
       <c r="U45"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>7</v>
       </c>
@@ -9546,7 +9555,7 @@
       </c>
       <c r="U46"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>7</v>
       </c>
@@ -9588,7 +9597,7 @@
       </c>
       <c r="U47"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>7</v>
       </c>
@@ -9627,7 +9636,7 @@
       </c>
       <c r="U48"/>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7</v>
       </c>
@@ -9666,7 +9675,7 @@
       </c>
       <c r="U49"/>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>7</v>
       </c>
@@ -9708,7 +9717,7 @@
       </c>
       <c r="U50"/>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>7</v>
       </c>
@@ -9747,7 +9756,7 @@
       </c>
       <c r="U51"/>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>7</v>
       </c>
@@ -9786,7 +9795,7 @@
       </c>
       <c r="U52"/>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>7</v>
       </c>
@@ -9828,7 +9837,7 @@
       </c>
       <c r="U53"/>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>7</v>
       </c>
@@ -9870,7 +9879,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>7</v>
       </c>
@@ -9909,7 +9918,7 @@
       </c>
       <c r="U55"/>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>7</v>
       </c>
@@ -9948,7 +9957,7 @@
       </c>
       <c r="U56"/>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>7</v>
       </c>
@@ -9987,7 +9996,7 @@
       </c>
       <c r="U57"/>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>7</v>
       </c>
@@ -10029,7 +10038,7 @@
       </c>
       <c r="U58"/>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>7</v>
       </c>
@@ -10068,7 +10077,7 @@
       </c>
       <c r="U59"/>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>7</v>
       </c>
@@ -10107,7 +10116,7 @@
       </c>
       <c r="U60"/>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>7</v>
       </c>
@@ -10146,7 +10155,7 @@
       </c>
       <c r="U61"/>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>7</v>
       </c>
@@ -10185,7 +10194,7 @@
       </c>
       <c r="U62"/>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>7</v>
       </c>
@@ -10224,7 +10233,7 @@
       </c>
       <c r="U63"/>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>7</v>
       </c>
@@ -10263,7 +10272,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>7</v>
       </c>
@@ -10305,7 +10314,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>7</v>
       </c>
@@ -10344,7 +10353,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>7</v>
       </c>
@@ -10383,7 +10392,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>7</v>
       </c>
@@ -10422,7 +10431,7 @@
       </c>
       <c r="U68"/>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>7</v>
       </c>
@@ -10461,7 +10470,7 @@
       </c>
       <c r="U69"/>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>7</v>
       </c>
@@ -10500,7 +10509,7 @@
       </c>
       <c r="U70"/>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>7</v>
       </c>
@@ -10539,7 +10548,7 @@
       </c>
       <c r="U71"/>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>7</v>
       </c>
@@ -10578,7 +10587,7 @@
       </c>
       <c r="U72"/>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>7</v>
       </c>
@@ -10617,7 +10626,7 @@
       </c>
       <c r="U73"/>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>7</v>
       </c>
@@ -10659,7 +10668,7 @@
       </c>
       <c r="U74"/>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>7</v>
       </c>
@@ -10701,7 +10710,7 @@
       </c>
       <c r="U75"/>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>7</v>
       </c>
@@ -10740,7 +10749,7 @@
       </c>
       <c r="U76"/>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>7</v>
       </c>
@@ -10779,7 +10788,7 @@
       </c>
       <c r="U77"/>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>7</v>
       </c>
@@ -10818,7 +10827,7 @@
       </c>
       <c r="U78"/>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>7</v>
       </c>
@@ -10857,7 +10866,7 @@
       </c>
       <c r="U79"/>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>7</v>
       </c>
@@ -10899,7 +10908,7 @@
       </c>
       <c r="U80"/>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>7</v>
       </c>
@@ -10938,7 +10947,7 @@
       </c>
       <c r="U81"/>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>7</v>
       </c>
@@ -10977,7 +10986,7 @@
       </c>
       <c r="U82"/>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>7</v>
       </c>
@@ -11019,7 +11028,7 @@
       </c>
       <c r="U83"/>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>7</v>
       </c>
@@ -11058,7 +11067,7 @@
       </c>
       <c r="U84"/>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>7</v>
       </c>
@@ -11097,7 +11106,7 @@
       </c>
       <c r="U85"/>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>7</v>
       </c>
@@ -11136,7 +11145,7 @@
       </c>
       <c r="U86"/>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>7</v>
       </c>
@@ -11175,7 +11184,7 @@
       </c>
       <c r="U87"/>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>7</v>
       </c>
@@ -11214,7 +11223,7 @@
       </c>
       <c r="U88"/>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>7</v>
       </c>
@@ -11253,7 +11262,7 @@
       </c>
       <c r="U89"/>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>7</v>
       </c>
@@ -11292,7 +11301,7 @@
       </c>
       <c r="U90"/>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>7</v>
       </c>
@@ -11331,7 +11340,7 @@
       </c>
       <c r="U91"/>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>7</v>
       </c>
@@ -11370,7 +11379,7 @@
       </c>
       <c r="U92"/>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>7</v>
       </c>
@@ -11409,7 +11418,7 @@
       </c>
       <c r="U93"/>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>7</v>
       </c>
@@ -11448,7 +11457,7 @@
       </c>
       <c r="U94"/>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>7</v>
       </c>
@@ -11490,7 +11499,7 @@
       </c>
       <c r="U95"/>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>7</v>
       </c>
@@ -11532,7 +11541,7 @@
       </c>
       <c r="U96"/>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>7</v>
       </c>
@@ -11571,7 +11580,7 @@
       </c>
       <c r="U97"/>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>7</v>
       </c>
@@ -11610,7 +11619,7 @@
       </c>
       <c r="U98"/>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>7</v>
       </c>
@@ -11652,7 +11661,7 @@
       </c>
       <c r="U99"/>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>7</v>
       </c>
@@ -11694,7 +11703,7 @@
       </c>
       <c r="U100"/>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>7</v>
       </c>
@@ -11733,7 +11742,7 @@
       </c>
       <c r="U101"/>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>7</v>
       </c>
@@ -11772,7 +11781,7 @@
       </c>
       <c r="U102"/>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>7</v>
       </c>
@@ -11814,7 +11823,7 @@
       </c>
       <c r="U103"/>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>7</v>
       </c>
@@ -11853,7 +11862,7 @@
       </c>
       <c r="U104"/>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>7</v>
       </c>
@@ -11892,7 +11901,7 @@
       </c>
       <c r="U105"/>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>7</v>
       </c>
@@ -11931,7 +11940,7 @@
       </c>
       <c r="U106"/>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>7</v>
       </c>
@@ -11970,7 +11979,7 @@
       </c>
       <c r="U107"/>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>7</v>
       </c>
@@ -12012,7 +12021,7 @@
       </c>
       <c r="U108"/>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>7</v>
       </c>
@@ -12051,7 +12060,7 @@
       </c>
       <c r="U109"/>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>7</v>
       </c>
@@ -12090,7 +12099,7 @@
       </c>
       <c r="U110"/>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>7</v>
       </c>
@@ -12129,7 +12138,7 @@
       </c>
       <c r="U111"/>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>7</v>
       </c>
@@ -12168,7 +12177,7 @@
       </c>
       <c r="U112"/>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>7</v>
       </c>
@@ -12207,7 +12216,7 @@
       </c>
       <c r="U113"/>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>7</v>
       </c>
@@ -12249,7 +12258,7 @@
       </c>
       <c r="U114"/>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>7</v>
       </c>
@@ -12291,7 +12300,7 @@
       </c>
       <c r="U115"/>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>7</v>
       </c>
@@ -12333,7 +12342,7 @@
       </c>
       <c r="U116"/>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>7</v>
       </c>
@@ -12372,7 +12381,7 @@
       </c>
       <c r="U117"/>
     </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>7</v>
       </c>
@@ -12411,7 +12420,7 @@
       </c>
       <c r="U118"/>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>7</v>
       </c>
@@ -12450,7 +12459,7 @@
       </c>
       <c r="U119"/>
     </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>7</v>
       </c>
@@ -12489,7 +12498,7 @@
       </c>
       <c r="U120"/>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>7</v>
       </c>
@@ -12528,7 +12537,7 @@
       </c>
       <c r="U121"/>
     </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>7</v>
       </c>
@@ -12567,7 +12576,7 @@
       </c>
       <c r="U122"/>
     </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>7</v>
       </c>
@@ -12606,7 +12615,7 @@
       </c>
       <c r="U123"/>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>7</v>
       </c>
@@ -12648,7 +12657,7 @@
       </c>
       <c r="U124"/>
     </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>7</v>
       </c>
@@ -12690,7 +12699,7 @@
       </c>
       <c r="U125"/>
     </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>7</v>
       </c>
@@ -12729,7 +12738,7 @@
       </c>
       <c r="U126"/>
     </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>7</v>
       </c>
@@ -12768,7 +12777,7 @@
       </c>
       <c r="U127"/>
     </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>7</v>
       </c>
@@ -12807,7 +12816,7 @@
       </c>
       <c r="U128"/>
     </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>7</v>
       </c>
@@ -12849,7 +12858,7 @@
       </c>
       <c r="U129"/>
     </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>7</v>
       </c>
@@ -12891,7 +12900,7 @@
       </c>
       <c r="U130"/>
     </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>7</v>
       </c>
@@ -12930,7 +12939,7 @@
       </c>
       <c r="U131"/>
     </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>7</v>
       </c>
@@ -12972,7 +12981,7 @@
       </c>
       <c r="U132"/>
     </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>7</v>
       </c>
@@ -12999,7 +13008,7 @@
       </c>
       <c r="U133"/>
     </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>7</v>
       </c>
@@ -13041,7 +13050,7 @@
       </c>
       <c r="U134"/>
     </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>7</v>
       </c>
@@ -13080,7 +13089,7 @@
       </c>
       <c r="U135"/>
     </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>7</v>
       </c>
@@ -13119,7 +13128,7 @@
       </c>
       <c r="U136"/>
     </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>7</v>
       </c>
@@ -13158,7 +13167,7 @@
       </c>
       <c r="U137"/>
     </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>7</v>
       </c>
@@ -13197,7 +13206,7 @@
       </c>
       <c r="U138"/>
     </row>
-    <row r="139" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>7</v>
       </c>
@@ -13239,7 +13248,7 @@
       </c>
       <c r="U139"/>
     </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>7</v>
       </c>
@@ -13278,7 +13287,7 @@
       </c>
       <c r="U140"/>
     </row>
-    <row r="141" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>7</v>
       </c>
@@ -13323,7 +13332,7 @@
       </c>
       <c r="U141"/>
     </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>7</v>
       </c>
@@ -13365,7 +13374,7 @@
       </c>
       <c r="U142"/>
     </row>
-    <row r="143" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>7</v>
       </c>
@@ -13404,7 +13413,7 @@
       </c>
       <c r="U143"/>
     </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>7</v>
       </c>
@@ -13443,7 +13452,7 @@
       </c>
       <c r="U144"/>
     </row>
-    <row r="145" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>7</v>
       </c>
@@ -13485,7 +13494,7 @@
       </c>
       <c r="U145"/>
     </row>
-    <row r="146" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>7</v>
       </c>
@@ -13527,7 +13536,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="147" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>7</v>
       </c>
@@ -13569,7 +13578,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="148" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>7</v>
       </c>
@@ -13608,7 +13617,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="149" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>7</v>
       </c>
@@ -13647,7 +13656,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="150" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>7</v>
       </c>
@@ -13772,22 +13781,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -13822,7 +13831,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -13855,7 +13864,7 @@
       </c>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -13888,7 +13897,7 @@
       </c>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -13921,7 +13930,7 @@
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -13956,7 +13965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -13989,7 +13998,7 @@
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>34</v>
       </c>
@@ -14022,7 +14031,7 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>35</v>
       </c>
@@ -14055,7 +14064,7 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>36</v>
       </c>
@@ -14088,7 +14097,7 @@
       </c>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>37</v>
       </c>
@@ -14121,7 +14130,7 @@
       </c>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -14154,7 +14163,7 @@
       </c>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
@@ -14187,7 +14196,7 @@
       </c>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
@@ -14222,7 +14231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>41</v>
       </c>
@@ -14257,7 +14266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -14292,7 +14301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
@@ -14325,7 +14334,7 @@
       </c>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>44</v>
       </c>
@@ -14358,7 +14367,7 @@
       </c>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>45</v>
       </c>
@@ -14391,7 +14400,7 @@
       </c>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>46</v>
       </c>
@@ -14426,7 +14435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>47</v>
       </c>
@@ -14461,7 +14470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
@@ -14496,7 +14505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>49</v>
       </c>
@@ -14531,7 +14540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>50</v>
       </c>
@@ -14564,7 +14573,7 @@
       </c>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>51</v>
       </c>
@@ -14599,7 +14608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>52</v>
       </c>
@@ -14632,7 +14641,7 @@
       </c>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>53</v>
       </c>
@@ -14667,7 +14676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>54</v>
       </c>
@@ -14702,7 +14711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>55</v>
       </c>
@@ -14735,7 +14744,7 @@
       </c>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>56</v>
       </c>
@@ -14770,7 +14779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>57</v>
       </c>
@@ -14805,7 +14814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>58</v>
       </c>
@@ -14840,7 +14849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>59</v>
       </c>
@@ -14875,7 +14884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>60</v>
       </c>
@@ -14910,7 +14919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>61</v>
       </c>
@@ -14943,7 +14952,7 @@
       </c>
       <c r="K34" s="6"/>
     </row>
-    <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>62</v>
       </c>
@@ -14978,7 +14987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>63</v>
       </c>
@@ -15013,7 +15022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>64</v>
       </c>
@@ -15048,7 +15057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>65</v>
       </c>
@@ -15083,7 +15092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>66</v>
       </c>
@@ -15118,7 +15127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>67</v>
       </c>
@@ -15151,7 +15160,7 @@
       </c>
       <c r="K40" s="6"/>
     </row>
-    <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>68</v>
       </c>
@@ -15184,7 +15193,7 @@
       </c>
       <c r="K41" s="6"/>
     </row>
-    <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>69</v>
       </c>
@@ -15217,7 +15226,7 @@
       </c>
       <c r="K42" s="6"/>
     </row>
-    <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>70</v>
       </c>
@@ -15252,7 +15261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>71</v>
       </c>
@@ -15287,7 +15296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>72</v>
       </c>
@@ -15322,7 +15331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>73</v>
       </c>
@@ -15355,7 +15364,7 @@
       </c>
       <c r="K46" s="6"/>
     </row>
-    <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>74</v>
       </c>
@@ -15388,7 +15397,7 @@
       </c>
       <c r="K47" s="6"/>
     </row>
-    <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>75</v>
       </c>
@@ -15421,7 +15430,7 @@
       </c>
       <c r="K48" s="6"/>
     </row>
-    <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>76</v>
       </c>
@@ -15456,7 +15465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>77</v>
       </c>
@@ -15489,7 +15498,7 @@
       </c>
       <c r="K50" s="6"/>
     </row>
-    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>78</v>
       </c>
@@ -15522,7 +15531,7 @@
       </c>
       <c r="K51" s="6"/>
     </row>
-    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>79</v>
       </c>
@@ -15555,7 +15564,7 @@
       </c>
       <c r="K52" s="6"/>
     </row>
-    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>80</v>
       </c>
@@ -15588,7 +15597,7 @@
       </c>
       <c r="K53" s="6"/>
     </row>
-    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>81</v>
       </c>
@@ -15611,7 +15620,7 @@
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
     </row>
-    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>82</v>
       </c>
@@ -15644,7 +15653,7 @@
       </c>
       <c r="K55" s="6"/>
     </row>
-    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>83</v>
       </c>

</xml_diff>